<commit_message>
Stored Procedure Aut. Fakturierung exkl. Gutschriften
</commit_message>
<xml_diff>
--- a/Arbeitsjournale/Arbeitsjournal Marina.xlsx
+++ b/Arbeitsjournale/Arbeitsjournal Marina.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maris\Google Drive\SemesterarbeitDB\Doks\Journal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maris\OneDrive\zbw\datenbanken\Modul 2\DBSemesterProject\Arbeitsjournale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B57DB9A-BACB-46E8-83E4-CF132762CCF0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{8B57DB9A-BACB-46E8-83E4-CF132762CCF0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{27BA4AE5-6429-452C-973B-530D48B947C0}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -27,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
-  <si>
-    <t>Arbeitsjournal Semesterarbeit</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name: Marina Scherrer</t>
   </si>
@@ -47,43 +45,13 @@
     <t>Besprechung</t>
   </si>
   <si>
-    <t>ERM skizzieren</t>
-  </si>
-  <si>
-    <t>Vorlage Dokumentation erstellt</t>
-  </si>
-  <si>
-    <t>ERM erstellt</t>
-  </si>
-  <si>
-    <t>Dokumentation: Kapitel 1, Verzeichnisse</t>
-  </si>
-  <si>
-    <t>ERM ergänzt</t>
-  </si>
-  <si>
-    <t>Dokumentation: Kapitel 2</t>
-  </si>
-  <si>
-    <t>DDL Kundenverwaltung</t>
-  </si>
-  <si>
     <t>Total Stunden</t>
   </si>
   <si>
-    <t>Versionierung</t>
+    <t>Arbeitsjournal Semesterarbeit, Modul 2</t>
   </si>
   <si>
-    <t>Dokumentation: Kapitel 3 + diverse Korrekturen</t>
-  </si>
-  <si>
-    <t>Telefonkonferenz</t>
-  </si>
-  <si>
-    <t>Fertigstellung Dokumentation</t>
-  </si>
-  <si>
-    <t>DML Kundenverwaltung</t>
+    <t>Stored Procedure BillPoD</t>
   </si>
 </sst>
 </file>
@@ -525,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -537,9 +505,9 @@
     <col min="7" max="26" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -597,7 +565,7 @@
     </row>
     <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -655,13 +623,13 @@
     </row>
     <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="C5" s="10" t="s">
         <v>3</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>4</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -689,13 +657,13 @@
     </row>
     <row r="6" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
-        <v>43321</v>
+        <v>43473</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -723,13 +691,13 @@
     </row>
     <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
-        <v>43328</v>
+        <v>43485</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -756,15 +724,9 @@
       <c r="Z7" s="5"/>
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
-        <v>43331</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="14">
-        <v>0.5</v>
-      </c>
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="14"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -790,15 +752,9 @@
       <c r="Z8" s="5"/>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
-        <v>43333</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="14">
-        <v>1.5</v>
-      </c>
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -824,15 +780,9 @@
       <c r="Z9" s="5"/>
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11">
-        <v>43335</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="13">
-        <v>1</v>
-      </c>
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -858,15 +808,9 @@
       <c r="Z10" s="5"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11">
-        <v>43335</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="13">
-        <v>1</v>
-      </c>
+      <c r="A11" s="11"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -892,15 +836,9 @@
       <c r="Z11" s="5"/>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11">
-        <v>43346</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="14">
-        <v>0.5</v>
-      </c>
+      <c r="A12" s="11"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -926,15 +864,9 @@
       <c r="Z12" s="5"/>
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11">
-        <v>43346</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="13">
-        <v>1</v>
-      </c>
+      <c r="A13" s="11"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -960,15 +892,9 @@
       <c r="Z13" s="5"/>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11">
-        <v>43346</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="13">
-        <v>1</v>
-      </c>
+      <c r="A14" s="11"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -994,15 +920,9 @@
       <c r="Z14" s="5"/>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11">
-        <v>43349</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="14">
-        <v>0.5</v>
-      </c>
+      <c r="A15" s="11"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -1028,15 +948,9 @@
       <c r="Z15" s="5"/>
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="20">
-        <v>43352</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="14">
-        <v>3</v>
-      </c>
+      <c r="A16" s="20"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="14"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -1062,15 +976,9 @@
       <c r="Z16" s="5"/>
     </row>
     <row r="17" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="20">
-        <v>43358</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="14">
-        <v>1.5</v>
-      </c>
+      <c r="A17" s="20"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="14"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -1096,15 +1004,9 @@
       <c r="Z17" s="5"/>
     </row>
     <row r="18" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="20">
-        <v>43358</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="14">
-        <v>1</v>
-      </c>
+      <c r="A18" s="20"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -1130,15 +1032,9 @@
       <c r="Z18" s="5"/>
     </row>
     <row r="19" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="20">
-        <v>43358</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="14">
-        <v>2.5</v>
-      </c>
+      <c r="A19" s="20"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -1669,12 +1565,12 @@
     </row>
     <row r="38" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="18" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B38" s="18"/>
       <c r="C38" s="19">
         <f>SUM(C6:C36)</f>
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>

</xml_diff>